<commit_message>
✨ feat: cpu 사용 옵션 추가 1. run.py, baseline.py의 config.yaml에서 cuda 불리안 옵션을 수정 2. inference.py (xie2019)의 커멘드 python baseline.py --no-cuda
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannibal\Desktop\cau_cats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12685B39-6A80-4EB4-ABC4-88A55F4C436B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8782AAC6-2A65-4003-99C5-502B040B45B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5470" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
   <sheets>
     <sheet name="연산량, 데이터셋 비교" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>모델</t>
   </si>
@@ -138,10 +138,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>샘플당 평균 Forward Pass 시간 (gpu 캐시 비우고,1장을 100번 반복측정 후 평균)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>데이터셋</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -244,6 +240,30 @@
   </si>
   <si>
     <t>run_20251108_121006_53</t>
+  </si>
+  <si>
+    <t>샘플당 평균 CPU Forward Pass 시간 (더미1장을 100번 반복측정 후 평균)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>샘플당 평균 GPU Forward Pass 시간 (gpu 캐시 비우고, 더미 1장을 100번 반복측정 후 평균)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/run_20251110_194054</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/run_efficientnet_b0_20251110_194550</t>
+  </si>
+  <si>
+    <t>log/Sewer-ML/run_mobilenet_v4_20251110_194752</t>
+  </si>
+  <si>
+    <t>log/Sewer-ML/run_resnet18_20251110_194424</t>
+  </si>
+  <si>
+    <t>inference_results</t>
   </si>
 </sst>
 </file>
@@ -712,29 +732,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A623D5-CCB0-4793-B626-CA6A042C8AFE}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="8" width="20.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="16.4140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="8" width="20.19921875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="61.796875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="102.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="102" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>19</v>
@@ -749,19 +770,22 @@
         <v>21</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>8</v>
@@ -777,15 +801,18 @@
         <v>11</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>23</v>
@@ -806,15 +833,21 @@
         <v>0.2</v>
       </c>
       <c r="I3" s="1">
+        <v>10.06</v>
+      </c>
+      <c r="J3" s="1">
         <v>65.77</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K3" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>23</v>
@@ -835,15 +868,21 @@
         <v>0.65</v>
       </c>
       <c r="I4" s="1">
+        <v>10.51</v>
+      </c>
+      <c r="J4" s="1">
         <v>203.42</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>23</v>
@@ -864,15 +903,21 @@
         <v>1.57</v>
       </c>
       <c r="I5" s="1">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="J5" s="1">
         <v>89.51</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="K5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -893,84 +938,102 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="I6" s="1">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="J6" s="1">
         <v>60.28</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
-        <v>39</v>
+      <c r="K6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="E7" s="6">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="E7" s="2">
         <v>29691</v>
       </c>
-      <c r="F7" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.18</v>
+      <c r="F7" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.84</v>
       </c>
       <c r="H7" s="1">
-        <v>0.71</v>
-      </c>
-      <c r="I7" s="5">
-        <v>19.38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="1">
+        <v>21.07</v>
+      </c>
+      <c r="J7" s="1">
+        <v>61.07</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="1">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="5">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="E8" s="6">
         <v>29691</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.42</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.84</v>
+      <c r="F8" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.18</v>
       </c>
       <c r="H8" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="I8" s="1">
-        <v>61.07</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>0.71</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.61</v>
+      </c>
+      <c r="J8" s="5">
+        <v>19.38</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="B15" s="7">
         <v>1040129</v>
@@ -982,9 +1045,9 @@
         <v>130046</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="7">
         <v>367</v>
@@ -996,9 +1059,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="7">
         <v>1353</v>
@@ -1010,19 +1073,19 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C22" s="2"/>
     </row>
   </sheetData>
@@ -1035,20 +1098,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED2E3D2-ADA8-4356-BFE1-6111EA273D35}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="C1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="8" width="20.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="16.4140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="40.75" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="8" width="20.19921875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.19921875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="40.69921875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1125,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
@@ -1083,7 +1146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1181,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1153,10 +1216,10 @@
         <v>0.90949999999999998</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1191,10 +1254,10 @@
         <v>0.9244</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1229,10 +1292,10 @@
         <v>0.91769999999999996</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1267,17 +1330,17 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
     </row>
@@ -1291,20 +1354,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083EF1A-8817-41A5-B7D4-F7B8AC6BEDDD}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="8" width="20.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="16.4140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="41.6640625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="8" width="20.19921875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.19921875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="41.69921875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1318,7 +1381,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
@@ -1339,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1374,7 +1437,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="20.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="20.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1409,10 +1472,10 @@
         <v>1</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1447,10 +1510,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1485,10 +1548,10 @@
         <v>0.9778</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1523,17 +1586,17 @@
         <v>0.97829999999999995</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
     </row>
@@ -1547,20 +1610,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="8" width="20.1640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="16.4140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="1" max="8" width="20.19921875" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.3984375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.19921875" style="1" customWidth="1"/>
     <col min="12" max="12" width="41.5" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.6640625" style="1"/>
+    <col min="13" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="61.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1574,7 +1637,7 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
@@ -1595,7 +1658,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1630,7 +1693,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1665,10 +1728,10 @@
         <v>0.91339999999999999</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1703,10 +1766,10 @@
         <v>0.91080000000000005</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1741,10 +1804,10 @@
         <v>0.89629999999999999</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1779,10 +1842,10 @@
         <v>0.86960000000000004</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="C8" s="2"/>
       <c r="D8" s="3"/>
     </row>

</xml_diff>

<commit_message>
🎨 refactor: Sewer-TAP, Sewer-TAPNEW 의 클래스 이름인 normal, abnormal에서도 F1_normal 그래프가 정상적으로 그려지도록 수정
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD27020-14AB-4806-948F-7CBDEC8E402A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967EE962-94DD-4873-B838-628236CF726C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
   <sheets>
     <sheet name="연산량, 데이터셋 비교" sheetId="4" r:id="rId1"/>
-    <sheet name="Sewer-ML" sheetId="1" r:id="rId2"/>
-    <sheet name="Sewer-TAP" sheetId="2" r:id="rId3"/>
-    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId4"/>
+    <sheet name="학습 레시피" sheetId="5" r:id="rId2"/>
+    <sheet name="Sewer-ML" sheetId="1" r:id="rId3"/>
+    <sheet name="Sewer-TAP" sheetId="2" r:id="rId4"/>
+    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
   <si>
     <t>모델</t>
   </si>
@@ -263,6 +264,52 @@
   </si>
   <si>
     <t>1epoch당 학습시간 (GPU 사용 기준)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resize, RandomHorizontalFlip, ColorJitter, Norm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pre_trained</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>optimizer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SGD Momentum</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdamW</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>scheduler</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>multisteplr</t>
+  </si>
+  <si>
+    <t>CosineAnnealingLR</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>preprocess</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -273,7 +320,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +361,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -334,7 +398,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -357,6 +421,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -366,7 +445,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -396,6 +475,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A623D5-CCB0-4793-B626-CA6A042C8AFE}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="93" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1095,11 +1198,192 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2844C75D-B20C-4DF4-8D50-5B6ECD2343AB}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="20.19921875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="43.69921875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="11" customWidth="1"/>
+    <col min="6" max="6" width="23.296875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" style="11" customWidth="1"/>
+    <col min="8" max="8" width="18.19921875" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="8.796875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10">
+        <v>90</v>
+      </c>
+      <c r="C2" s="12">
+        <v>3244244</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="13">
+        <v>256</v>
+      </c>
+      <c r="F2" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="15">
+        <v>90</v>
+      </c>
+      <c r="C3" s="16">
+        <v>3244244</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="17">
+        <v>256</v>
+      </c>
+      <c r="F3" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="15">
+        <v>90</v>
+      </c>
+      <c r="C4" s="16">
+        <v>3244244</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="17">
+        <v>256</v>
+      </c>
+      <c r="F4" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="15">
+        <v>90</v>
+      </c>
+      <c r="C5" s="16">
+        <v>3244244</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="17">
+        <v>256</v>
+      </c>
+      <c r="F5" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="A6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15">
+        <v>90</v>
+      </c>
+      <c r="C6" s="16">
+        <v>3244244</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="17">
+        <v>256</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED2E3D2-ADA8-4356-BFE1-6111EA273D35}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="77" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="77" workbookViewId="0">
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1113,7 +1397,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="61.2" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>12</v>
@@ -1150,8 +1434,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
+      <c r="B2" s="1">
+        <v>90</v>
       </c>
       <c r="C2" s="2">
         <v>3244244</v>
@@ -1350,7 +1634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083EF1A-8817-41A5-B7D4-F7B8AC6BEDDD}">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -1606,7 +1890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
   <dimension ref="A1:L8"/>
   <sheetViews>

</xml_diff>

<commit_message>
✨ feat: CrossEntropyLoss, BCEWithLogitsLoss 옵션 추가 BCEWithLogitsLoss의 pos_weight=defect/normal, abnormal/normal 자동계산 추가
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73EDCBD-2DA1-4D0B-8906-D7B8260F7000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59F236-C3C6-4FCE-AA9D-E2FEFB6347FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
   <sheets>
     <sheet name="연산량, 데이터셋 비교" sheetId="4" r:id="rId1"/>
-    <sheet name="학습 레시피" sheetId="5" r:id="rId2"/>
+    <sheet name="recipe" sheetId="5" r:id="rId2"/>
     <sheet name="Sewer-ML" sheetId="1" r:id="rId3"/>
     <sheet name="Sewer-TAP" sheetId="2" r:id="rId4"/>
     <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId5"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="149">
   <si>
     <t>모델</t>
   </si>
@@ -298,10 +298,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>11.18</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Final epoch’s Loss (train mode)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -426,32 +422,16 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>64</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>90</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>run_resnet18_20251108_125319_60</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.0023</t>
   </si>
   <si>
-    <t>run_efficientnet_b0_20251108_135948_61</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.0232</t>
   </si>
   <si>
-    <t>run_mobilenet_v4_20251108_163343_62</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.0811</t>
   </si>
   <si>
@@ -499,6 +479,124 @@
   </si>
   <si>
     <t>BCEWithLogitsLoss(pos_weight = neg_count/pos_count)</t>
+  </si>
+  <si>
+    <t>BCEWithLogitsLoss(pos_weight = neg_count/pos_count)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>99.97</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0019</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>91.90</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9351</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9098</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9222</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9020</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9293</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9154</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8870</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8820</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8750</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/baseline_resnet18_20251111_153058</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/baseline_efficientnet_b0_20251111_153240</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/baseline_mobilenet_v4_20251112_113929</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sewer-TAPNEW log</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal/Defect</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>normal/abnormal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>552820 / 487309</t>
+  </si>
+  <si>
+    <t>log/run_resnet18_20251108_125319_60</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/run_efficientnet_b0_20251108_135948_61</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/run_mobilenet_v4_20251108_163343_62</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CosineAnnealingLR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.12-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdamW, Cosine 이것도 각각 수정하고 변형 필요</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -509,7 +607,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,6 +674,23 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -628,7 +743,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -694,6 +809,33 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1033,7 +1175,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1133,7 +1275,7 @@
       <c r="I3" s="15">
         <v>10.06</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="28">
         <v>65.77</v>
       </c>
       <c r="K3" s="15" t="s">
@@ -1168,7 +1310,7 @@
       <c r="I4" s="15">
         <v>10.51</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="28">
         <v>203.42</v>
       </c>
       <c r="K4" s="15" t="s">
@@ -1203,7 +1345,7 @@
       <c r="I5" s="15">
         <v>17.559999999999999</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="28">
         <v>89.51</v>
       </c>
       <c r="K5" s="15" t="s">
@@ -1238,7 +1380,7 @@
       <c r="I6" s="15">
         <v>8.9600000000000009</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="28">
         <v>60.28</v>
       </c>
       <c r="K6" s="15" t="s">
@@ -1273,7 +1415,7 @@
       <c r="I7" s="15">
         <v>21.07</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="28">
         <v>61.07</v>
       </c>
       <c r="K7" s="15" t="s">
@@ -1308,7 +1450,7 @@
       <c r="I8" s="17">
         <v>3.61</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="29">
         <v>19.38</v>
       </c>
       <c r="K8" s="15" t="s">
@@ -1328,6 +1470,12 @@
       <c r="D14" s="14" t="s">
         <v>32</v>
       </c>
+      <c r="E14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
@@ -1342,6 +1490,12 @@
       <c r="D15" s="19">
         <v>130046</v>
       </c>
+      <c r="E15" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
@@ -1356,8 +1510,11 @@
       <c r="D16" s="19">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E16" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
@@ -1370,20 +1527,23 @@
       <c r="D17" s="19">
         <v>339</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E17" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C18" s="16"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C19" s="16"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C21" s="16"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="C22" s="16"/>
     </row>
   </sheetData>
@@ -1394,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2844C75D-B20C-4DF4-8D50-5B6ECD2343AB}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1406,7 +1566,7 @@
     <col min="2" max="2" width="11.796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="43.69921875" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.69921875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.09765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="51.8984375" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.3984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="23.296875" style="2" customWidth="1"/>
     <col min="8" max="8" width="18.296875" style="2" customWidth="1"/>
@@ -1433,7 +1593,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -1450,10 +1610,10 @@
     </row>
     <row r="3" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>57</v>
@@ -1462,7 +1622,7 @@
         <v>256</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F3" s="7">
         <v>90</v>
@@ -1482,22 +1642,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>102</v>
+      <c r="D4" s="30">
+        <v>64</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F4" s="9">
         <v>90</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>61</v>
@@ -1511,22 +1671,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>102</v>
+      <c r="D5" s="30">
+        <v>64</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F5" s="9">
         <v>90</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>61</v>
@@ -1540,22 +1700,22 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>102</v>
+      <c r="D6" s="30">
+        <v>64</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F6" s="9">
         <v>90</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>61</v>
@@ -1569,22 +1729,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>102</v>
+      <c r="D7" s="30">
+        <v>64</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F7" s="9">
         <v>90</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>61</v>
@@ -1594,8 +1754,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="2">
-        <v>11.18</v>
+      <c r="A10" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -1612,7 +1772,7 @@
         <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>12</v>
@@ -1629,10 +1789,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>57</v>
@@ -1641,7 +1801,7 @@
         <v>256</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F12" s="7">
         <v>90</v>
@@ -1661,7 +1821,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>57</v>
@@ -1669,7 +1829,9 @@
       <c r="D13" s="10">
         <v>256</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="F13" s="9">
         <v>90</v>
       </c>
@@ -1688,7 +1850,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>57</v>
@@ -1696,7 +1858,9 @@
       <c r="D14" s="10">
         <v>256</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="F14" s="9">
         <v>90</v>
       </c>
@@ -1715,7 +1879,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>57</v>
@@ -1723,7 +1887,9 @@
       <c r="D15" s="10">
         <v>256</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="F15" s="9">
         <v>90</v>
       </c>
@@ -1742,7 +1908,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>57</v>
@@ -1751,7 +1917,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F16" s="9">
         <v>90</v>
@@ -1763,7 +1929,202 @@
         <v>61</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>64</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="8">
+        <v>256</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="7">
+        <v>90</v>
+      </c>
+      <c r="G21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="10">
+        <v>256</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="9">
+        <v>90</v>
+      </c>
+      <c r="G22" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="10">
+        <v>256</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="9">
+        <v>90</v>
+      </c>
+      <c r="G23" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="10">
+        <v>256</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="9">
+        <v>90</v>
+      </c>
+      <c r="G24" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="10">
+        <v>256</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="9">
+        <v>90</v>
+      </c>
+      <c r="G25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="E29" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1774,19 +2135,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED2E3D2-ADA8-4356-BFE1-6111EA273D35}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="9" width="20.19921875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="17.59765625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="19.09765625" style="11" customWidth="1"/>
     <col min="11" max="11" width="16.3984375" style="11" customWidth="1"/>
     <col min="12" max="12" width="15.19921875" style="11" customWidth="1"/>
-    <col min="13" max="13" width="49.3984375" style="11" customWidth="1"/>
+    <col min="13" max="13" width="19.09765625" style="22" customWidth="1"/>
     <col min="14" max="16384" width="8.69921875" style="11"/>
   </cols>
   <sheetData>
@@ -1806,7 +2167,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>25</v>
@@ -1832,6 +2193,7 @@
       <c r="L2" s="20" t="s">
         <v>18</v>
       </c>
+      <c r="M2" s="23"/>
     </row>
     <row r="3" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
@@ -1841,7 +2203,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>23</v>
@@ -1870,6 +2232,7 @@
       <c r="L3" s="20">
         <v>0.90300000000000002</v>
       </c>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
@@ -1879,10 +2242,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E4" s="11">
         <v>99.93</v>
@@ -1908,8 +2271,8 @@
       <c r="L4" s="11">
         <v>0.90949999999999998</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>104</v>
+      <c r="M4" s="22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -1920,10 +2283,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E5" s="11">
         <v>99.09</v>
@@ -1949,8 +2312,8 @@
       <c r="L5" s="12">
         <v>0.9244</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>106</v>
+      <c r="M5" s="22" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -1961,10 +2324,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E6" s="11">
         <v>96.86</v>
@@ -1990,8 +2353,8 @@
       <c r="L6" s="11">
         <v>0.91769999999999996</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>108</v>
+      <c r="M6" s="22" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -2002,10 +2365,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E7" s="13">
         <v>90.93</v>
@@ -2031,157 +2394,195 @@
       <c r="L7" s="13">
         <v>0.90900000000000003</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="11" t="s">
+      <c r="M7" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A11" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="E11" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="23"/>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="20">
+        <v>90</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="20">
-        <v>90</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="20">
+        <v>23</v>
+      </c>
+      <c r="F12" s="20">
         <v>90.71</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G12" s="20">
         <v>0.92359999999999998</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H12" s="20">
         <v>0.8982</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I12" s="20">
         <v>0.91080000000000005</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J12" s="20">
         <v>0.88949999999999996</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K12" s="20">
         <v>0.91690000000000005</v>
       </c>
-      <c r="L13" s="20">
+      <c r="L12" s="20">
         <v>0.90300000000000002</v>
+      </c>
+      <c r="M12" s="23"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="22" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
+        <v>71</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="H20" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2191,10 +2592,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083EF1A-8817-41A5-B7D4-F7B8AC6BEDDD}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2202,7 +2603,7 @@
     <col min="1" max="9" width="20.19921875" style="1" customWidth="1"/>
     <col min="10" max="11" width="16.3984375" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="41.69921875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.59765625" style="24" customWidth="1"/>
     <col min="14" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
@@ -2222,7 +2623,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>25</v>
@@ -2248,6 +2649,7 @@
       <c r="L2" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -2295,10 +2697,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E4" s="1">
         <v>100</v>
@@ -2324,7 +2726,7 @@
       <c r="L4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -2336,10 +2738,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E5" s="1">
         <v>100</v>
@@ -2365,7 +2767,7 @@
       <c r="L5" s="1">
         <v>1</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2377,10 +2779,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1">
         <v>100</v>
@@ -2406,7 +2808,7 @@
       <c r="L6" s="1">
         <v>0.9778</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="24" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2418,10 +2820,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1">
         <v>98.64</v>
@@ -2447,137 +2849,134 @@
       <c r="L7" s="1">
         <v>0.97829999999999995</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="24" t="s">
         <v>47</v>
       </c>
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A12" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.55" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="20.55" customHeight="1" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="D16" s="1"/>
+      <c r="M16" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2587,18 +2986,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="9" width="20.19921875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="16.3984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.3984375" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="54.8984375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="24" customWidth="1"/>
     <col min="14" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
@@ -2618,7 +3018,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>25</v>
@@ -2644,6 +3044,7 @@
       <c r="L2" s="21" t="s">
         <v>18</v>
       </c>
+      <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
@@ -2691,10 +3092,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E4" s="5">
         <v>99.85</v>
@@ -2705,8 +3106,8 @@
       <c r="G4" s="5">
         <v>0.94579999999999997</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.88700000000000001</v>
+      <c r="H4" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="I4" s="1">
         <v>0.91549999999999998</v>
@@ -2720,7 +3121,7 @@
       <c r="L4" s="5">
         <v>0.91339999999999999</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="24" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2732,10 +3133,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E5" s="5">
         <v>99.85</v>
@@ -2761,7 +3162,7 @@
       <c r="L5" s="1">
         <v>0.91080000000000005</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="24" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2773,13 +3174,13 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" s="1">
-        <v>98.3</v>
+        <v>113</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="F6" s="1">
         <v>89.97</v>
@@ -2802,8 +3203,8 @@
       <c r="L6" s="1">
         <v>0.89629999999999999</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>119</v>
+      <c r="M6" s="24" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -2814,10 +3215,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E7" s="1">
         <v>91.65</v>
@@ -2828,14 +3229,14 @@
       <c r="G7" s="1">
         <v>0.87709999999999999</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0.875</v>
+      <c r="H7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="K7" s="1">
         <v>0.86419999999999997</v>
@@ -2843,248 +3244,396 @@
       <c r="L7" s="1">
         <v>0.86960000000000004</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="24" t="s">
         <v>48</v>
       </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A12" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K12" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="21" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>88.67</v>
+      </c>
+      <c r="F12" s="1">
+        <v>84.37</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>23</v>
+        <v>71</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.21440000000000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>90.94</v>
+      </c>
+      <c r="F13" s="1">
+        <v>84.37</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>23</v>
+        <v>74</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>23</v>
+        <v>81</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="1">
-        <v>0.30220000000000002</v>
-      </c>
       <c r="E14" s="1">
-        <v>88.67</v>
+        <v>91.09</v>
       </c>
       <c r="F14" s="1">
         <v>84.37</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>74</v>
+      <c r="G14" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.21440000000000001</v>
-      </c>
-      <c r="E15" s="1">
-        <v>90.94</v>
-      </c>
-      <c r="F15" s="1">
-        <v>84.37</v>
+        <v>71</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A19" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="25"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>90</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>90</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B23" s="1">
         <v>90</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="1">
-        <v>91.09</v>
-      </c>
-      <c r="F16" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="1">
         <v>90</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>90</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>100</v>
-      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="J16 I17" numberStoredAsText="1"/>
+    <ignoredError sqref="J14 I15" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
✨ feat: seed넘버를 global_seed 로 통합
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF59F236-C3C6-4FCE-AA9D-E2FEFB6347FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C7C58F-AE50-43BB-84B0-DEAA328F1C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
+    <workbookView xWindow="11028" yWindow="25812" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
   <sheets>
     <sheet name="연산량, 데이터셋 비교" sheetId="4" r:id="rId1"/>
     <sheet name="recipe" sheetId="5" r:id="rId2"/>
-    <sheet name="Sewer-ML" sheetId="1" r:id="rId3"/>
-    <sheet name="Sewer-TAP" sheetId="2" r:id="rId4"/>
-    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId5"/>
+    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId3"/>
+    <sheet name="Sewer-ML" sheetId="1" r:id="rId4"/>
+    <sheet name="Sewer-TAP" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="199">
   <si>
     <t>모델</t>
   </si>
@@ -294,10 +294,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>11.10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Final epoch’s Loss (train mode)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -386,38 +382,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0.1755</t>
-  </si>
-  <si>
-    <t>92.81</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>85.25</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8223</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9153</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8663</t>
-  </si>
-  <si>
-    <t>0.8944</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.7840</t>
-  </si>
-  <si>
-    <t>0.8355</t>
-  </si>
-  <si>
     <t>True</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -485,10 +449,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>11.12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>99.97</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -592,11 +552,233 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>11.12-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AdamW, Cosine 이것도 각각 수정하고 변형 필요</t>
+    <t>86.14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프리트레인드를 끄니까 베이스라인 성능이 감소했다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8333</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8765</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2142</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>91.56</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8927</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8869</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8638</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8363</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8827</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8589</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1616</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>92.89</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>86.73</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8367</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9266</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8794</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9091</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8025</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8525</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ours (t_max90)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_efficientnet_b0_20251112_120819</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_mobilenet_v4_20251112_120835</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_resnet18_20251112_120810</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_111331</t>
+  </si>
+  <si>
+    <t>0.371</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.83</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>89.38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8876</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8901</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8793</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1970</t>
+  </si>
+  <si>
+    <t>92.66</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.91</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8644</t>
+  </si>
+  <si>
+    <t>0.8644</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8519</t>
+  </si>
+  <si>
+    <t>0.3726</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>81.56</t>
+  </si>
+  <si>
+    <t>82.30</t>
+  </si>
+  <si>
+    <t>0.8383</t>
+  </si>
+  <si>
+    <t>0.7910</t>
+  </si>
+  <si>
+    <t>0.8140</t>
+  </si>
+  <si>
+    <t>0.7849</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8084</t>
+  </si>
+  <si>
+    <t>0.1681</t>
+  </si>
+  <si>
+    <t>93.43</t>
+  </si>
+  <si>
+    <t>92.19</t>
+  </si>
+  <si>
+    <t>0.9313</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9199</t>
+  </si>
+  <si>
+    <t>0.9256</t>
+  </si>
+  <si>
+    <t>0.9116</t>
+  </si>
+  <si>
+    <t>0.9241</t>
+  </si>
+  <si>
+    <t>0.9178</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_resnet18_20251112_134302</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_efficientnet_b0_20251112_134706</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_mobilenet_v4_20251112_134313</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1175,7 +1357,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1471,10 +1653,10 @@
         <v>32</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1491,10 +1673,10 @@
         <v>130046</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -1511,7 +1693,7 @@
         <v>92</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
@@ -1528,7 +1710,7 @@
         <v>339</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
@@ -1554,10 +1736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2844C75D-B20C-4DF4-8D50-5B6ECD2343AB}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A12" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1576,7 +1758,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
@@ -1593,7 +1775,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -1610,10 +1792,10 @@
     </row>
     <row r="3" spans="1:9" ht="20.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>57</v>
@@ -1622,7 +1804,7 @@
         <v>256</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F3" s="7">
         <v>90</v>
@@ -1642,7 +1824,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>57</v>
@@ -1651,13 +1833,13 @@
         <v>64</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F4" s="9">
         <v>90</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>61</v>
@@ -1671,7 +1853,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>57</v>
@@ -1680,13 +1862,13 @@
         <v>64</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F5" s="9">
         <v>90</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>61</v>
@@ -1700,7 +1882,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>57</v>
@@ -1709,13 +1891,13 @@
         <v>64</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F6" s="9">
         <v>90</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>61</v>
@@ -1729,7 +1911,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>57</v>
@@ -1738,13 +1920,13 @@
         <v>64</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F7" s="9">
         <v>90</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>61</v>
@@ -1755,7 +1937,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -1772,7 +1954,7 @@
         <v>65</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>12</v>
@@ -1789,10 +1971,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>57</v>
@@ -1801,7 +1983,7 @@
         <v>256</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F12" s="7">
         <v>90</v>
@@ -1821,7 +2003,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>57</v>
@@ -1830,7 +2012,7 @@
         <v>256</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F13" s="9">
         <v>90</v>
@@ -1850,7 +2032,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>57</v>
@@ -1859,7 +2041,7 @@
         <v>256</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F14" s="9">
         <v>90</v>
@@ -1879,7 +2061,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>57</v>
@@ -1888,7 +2070,7 @@
         <v>256</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F15" s="9">
         <v>90</v>
@@ -1908,7 +2090,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>57</v>
@@ -1917,7 +2099,7 @@
         <v>256</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F16" s="9">
         <v>90</v>
@@ -1929,7 +2111,7 @@
         <v>61</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
@@ -1945,7 +2127,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>147</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
@@ -1962,7 +2144,7 @@
         <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>12</v>
@@ -1979,10 +2161,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>57</v>
@@ -1991,7 +2173,7 @@
         <v>256</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="F21" s="7">
         <v>90</v>
@@ -2011,7 +2193,7 @@
         <v>3</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>57</v>
@@ -2020,7 +2202,7 @@
         <v>256</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F22" s="9">
         <v>90</v>
@@ -2040,7 +2222,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>57</v>
@@ -2049,7 +2231,7 @@
         <v>256</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F23" s="9">
         <v>90</v>
@@ -2069,7 +2251,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>57</v>
@@ -2078,7 +2260,7 @@
         <v>256</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F24" s="9">
         <v>90</v>
@@ -2098,7 +2280,7 @@
         <v>5</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>57</v>
@@ -2107,7 +2289,7 @@
         <v>256</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="F25" s="9">
         <v>90</v>
@@ -2119,12 +2301,365 @@
         <v>61</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E29" s="2" t="s">
-        <v>148</v>
+      <c r="A29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="8">
+        <v>256</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="7">
+        <v>90</v>
+      </c>
+      <c r="G30" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="10">
+        <v>256</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="9">
+        <v>90</v>
+      </c>
+      <c r="G31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="10">
+        <v>256</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="9">
+        <v>90</v>
+      </c>
+      <c r="G32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="10">
+        <v>256</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="9">
+        <v>90</v>
+      </c>
+      <c r="G33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="10">
+        <v>256</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="9">
+        <v>90</v>
+      </c>
+      <c r="G34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A38" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" s="8">
+        <v>256</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" s="7">
+        <v>90</v>
+      </c>
+      <c r="G39" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A40" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40" s="10">
+        <v>256</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="9">
+        <v>90</v>
+      </c>
+      <c r="G40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A41" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="10">
+        <v>256</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="9">
+        <v>90</v>
+      </c>
+      <c r="G41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A42" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="10">
+        <v>256</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" s="9">
+        <v>90</v>
+      </c>
+      <c r="G42" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A43" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="10">
+        <v>256</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="9">
+        <v>90</v>
+      </c>
+      <c r="G43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2134,11 +2669,1190 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
+  <dimension ref="A1:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="9" width="20.19921875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.3984375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" style="24" customWidth="1"/>
+    <col min="14" max="16384" width="8.69921875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="25"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="5">
+        <v>99.85</v>
+      </c>
+      <c r="F4" s="5">
+        <v>91.45</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.94579999999999997</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.88439999999999996</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.94440000000000002</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.91339999999999999</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>60</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="5">
+        <v>99.85</v>
+      </c>
+      <c r="F5" s="5">
+        <v>91.45</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.92049999999999998</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.9153</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.91779999999999995</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.91359999999999997</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" s="1">
+        <v>89.97</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.9133</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.89270000000000005</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.88549999999999995</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.90739999999999998</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.89629999999999999</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="1">
+        <v>91.65</v>
+      </c>
+      <c r="F7" s="1">
+        <v>87.61</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.87709999999999999</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.86960000000000004</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="25"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>90</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="E12" s="1">
+        <v>88.67</v>
+      </c>
+      <c r="F12" s="1">
+        <v>84.37</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1">
+        <v>90</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.21440000000000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>90.94</v>
+      </c>
+      <c r="F13" s="1">
+        <v>84.37</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>90</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1">
+        <v>91.09</v>
+      </c>
+      <c r="F14" s="1">
+        <v>84.37</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
+        <v>90</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M15" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="D16" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A21" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="25"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>90</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M23" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1">
+        <v>90</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1">
+        <v>90</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="1">
+        <v>90</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A30" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="25"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="1">
+        <v>90</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <v>90</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M33" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="1">
+        <v>90</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M34" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="1">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M35" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A39" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="L39" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="M39" s="25"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1">
+        <v>90</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M41" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
+        <v>90</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M42" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1">
+        <v>90</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M43" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" s="1">
+        <v>90</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M44" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="J14" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED2E3D2-ADA8-4356-BFE1-6111EA273D35}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2153,7 +3867,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -2167,7 +3881,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>25</v>
@@ -2203,7 +3917,7 @@
         <v>90</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>23</v>
@@ -2242,10 +3956,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E4" s="11">
         <v>99.93</v>
@@ -2272,7 +3986,7 @@
         <v>0.90949999999999998</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -2283,10 +3997,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E5" s="11">
         <v>99.09</v>
@@ -2313,7 +4027,7 @@
         <v>0.9244</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -2324,10 +4038,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E6" s="11">
         <v>96.86</v>
@@ -2354,7 +4068,7 @@
         <v>0.91769999999999996</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -2365,10 +4079,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="E7" s="13">
         <v>90.93</v>
@@ -2395,12 +4109,12 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
-        <v>120</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -2414,7 +4128,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>25</v>
@@ -2450,7 +4164,7 @@
         <v>90</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>23</v>
@@ -2486,40 +4200,40 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F13" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" s="22" t="s">
         <v>123</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="M13" s="22" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -2527,20 +4241,40 @@
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
+        <v>70</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="M14" s="22" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -2548,13 +4282,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
@@ -2562,10 +4296,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
@@ -2590,12 +4324,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083EF1A-8817-41A5-B7D4-F7B8AC6BEDDD}">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2609,7 +4343,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -2623,7 +4357,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>25</v>
@@ -2697,10 +4431,10 @@
         <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1">
         <v>100</v>
@@ -2738,10 +4472,10 @@
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1">
         <v>100</v>
@@ -2779,10 +4513,10 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="E6" s="1">
         <v>100</v>
@@ -2820,10 +4554,10 @@
         <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E7" s="1">
         <v>98.64</v>
@@ -2864,7 +4598,7 @@
         <v>24</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>25</v>
@@ -2935,10 +4669,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
@@ -2946,10 +4680,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -2957,10 +4691,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -2968,10 +4702,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.4">
@@ -2982,658 +4716,4 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
-  <dimension ref="A1:M24"/>
-  <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="9" width="20.19921875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.3984375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20" style="24" customWidth="1"/>
-    <col min="14" max="16384" width="8.69921875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>60</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="5">
-        <v>99.85</v>
-      </c>
-      <c r="F4" s="5">
-        <v>91.45</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.94579999999999997</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0.91549999999999998</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.88439999999999996</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.94440000000000002</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0.91339999999999999</v>
-      </c>
-      <c r="M4" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1">
-        <v>60</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="5">
-        <v>99.85</v>
-      </c>
-      <c r="F5" s="5">
-        <v>91.45</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.92049999999999998</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.9153</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.91779999999999995</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0.91359999999999997</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0.91080000000000005</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>60</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="1">
-        <v>89.97</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.9133</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.89270000000000005</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.90290000000000004</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0.88549999999999995</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0.90739999999999998</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0.89629999999999999</v>
-      </c>
-      <c r="M6" s="24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>60</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="1">
-        <v>91.65</v>
-      </c>
-      <c r="F7" s="1">
-        <v>87.61</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.87709999999999999</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.86419999999999997</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0.86960000000000004</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A10" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="25"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>90</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.30220000000000002</v>
-      </c>
-      <c r="E12" s="1">
-        <v>88.67</v>
-      </c>
-      <c r="F12" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1">
-        <v>90</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.21440000000000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>90.94</v>
-      </c>
-      <c r="F13" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1">
-        <v>90</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="1">
-        <v>91.09</v>
-      </c>
-      <c r="F14" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1">
-        <v>90</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M15" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A19" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M19" s="25"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1">
-        <v>90</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1">
-        <v>90</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="1">
-        <v>90</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1">
-        <v>90</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="J14 I15" numberStoredAsText="1"/>
-  </ignoredErrors>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
🎨 refactor: Sewer-ML 데이터 BCEloss의 pos_weight 계산 기능 호환 추가
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C7C58F-AE50-43BB-84B0-DEAA328F1C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA36E763-7755-4E60-9BED-ACC9FCC9010F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11028" yWindow="25812" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
   <sheets>
     <sheet name="연산량, 데이터셋 비교" sheetId="4" r:id="rId1"/>
     <sheet name="recipe" sheetId="5" r:id="rId2"/>
-    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId3"/>
-    <sheet name="Sewer-ML" sheetId="1" r:id="rId4"/>
-    <sheet name="Sewer-TAP" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="Sewer-TAPNEW" sheetId="3" r:id="rId4"/>
+    <sheet name="Sewer-ML" sheetId="1" r:id="rId5"/>
+    <sheet name="Sewer-TAP" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="239">
   <si>
     <t>모델</t>
   </si>
@@ -339,6 +340,9 @@
   </si>
   <si>
     <t>0.8642</t>
+  </si>
+  <si>
+    <t>0.8642</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -449,42 +453,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>99.97</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.0019</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>91.90</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9351</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9098</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9222</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9020</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9293</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9154</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.8870</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -501,18 +469,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>log/Sewer-ML/baseline_resnet18_20251111_153058</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>log/Sewer-ML/baseline_efficientnet_b0_20251111_153240</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>log/Sewer-ML/baseline_mobilenet_v4_20251112_113929</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Sewer-TAPNEW log</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -552,11 +508,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>86.14</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>프리트레인드를 끄니까 베이스라인 성능이 감소했다.</t>
+    <t>0.8916</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8757</t>
+  </si>
+  <si>
+    <t>0.8757</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -568,74 +527,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0.2142</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>91.56</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>0.8927</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>0.8869</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8638</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8363</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8827</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8589</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.1616</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>92.89</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>86.73</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8367</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9266</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8794</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9091</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8025</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.8525</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Ours (t_max90)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -649,9 +544,6 @@
     <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_resnet18_20251112_120810</t>
   </si>
   <si>
-    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_111331</t>
-  </si>
-  <si>
     <t>0.371</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -723,45 +615,6 @@
     <t>0.8084</t>
   </si>
   <si>
-    <t>0.1681</t>
-  </si>
-  <si>
-    <t>93.43</t>
-  </si>
-  <si>
-    <t>92.19</t>
-  </si>
-  <si>
-    <t>0.9313</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.9199</t>
-  </si>
-  <si>
-    <t>0.9256</t>
-  </si>
-  <si>
-    <t>0.9116</t>
-  </si>
-  <si>
-    <t>0.9241</t>
-  </si>
-  <si>
-    <t>0.9178</t>
-  </si>
-  <si>
-    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_resnet18_20251112_134302</t>
-  </si>
-  <si>
-    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_efficientnet_b0_20251112_134706</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_mobilenet_v4_20251112_134313</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -778,8 +631,291 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>log/Sewer-ML/run_20251113_002452</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_resnet18_20251112_150032</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_mobilenet_v4_20251112_150108</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_efficientnet_b0_20251112_150047</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_152742</t>
+  </si>
+  <si>
+    <t>0.0463</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>98.52</t>
+  </si>
+  <si>
+    <t>88.20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9006</t>
+  </si>
+  <si>
+    <t>0.8701</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8851</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8631</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8951</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8788</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0025</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>99.92</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9172</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8960</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8706</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9136</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.0178</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>99.38</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>86.43</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9119</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8222</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.8655</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1657</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>93.12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>87.02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_160430</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_160457</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_160546</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_160603</t>
+  </si>
+  <si>
+    <t>  dropout: 0.01</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251112_235548</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  dropout: 0.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  dropout: 0.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_002239</t>
+  </si>
+  <si>
+    <t>  decoder_ff_ratio: 3</t>
+  </si>
+  <si>
+    <t>run  lr: 0.1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>run  lr: 0.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원본 (run  lr: 0.001, dropout0.1, ff_ratio:2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  dropout: 0.01 2차 시도</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  decoder_ff_ratio: 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_005207</t>
+  </si>
+  <si>
+    <t>  dropout: 0.005</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_005347</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_012808</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_012839</t>
+  </si>
+  <si>
+    <t>ff_ratio3,  dropout: 0.01, run  lr: 0.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ff_ratio3, dropout: 0.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropout: 0.01, run  lr: 0.01</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_015857</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_021519</t>
+  </si>
+  <si>
+    <t>  decoder_ff_ratio: 4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  dropout: 0.05</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_033000</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_033014</t>
+  </si>
+  <si>
+    <t>  dropout: 0.05, res_attn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>위는 eta_min: 0.000001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>  dropout: 0.01, eta_min: 0.00001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_040357</t>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_040442</t>
+  </si>
+  <si>
+    <t>  dropout: 0.01, eta_min: 0.0001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dropout: 0.01. head3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_043630</t>
+  </si>
+  <si>
+    <t>dropout: 0.01. head1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251113_043740</t>
+  </si>
+  <si>
+    <t>0.2280</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>90.99</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>91.29</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9093</t>
+  </si>
+  <si>
+    <t>0.9169</t>
+  </si>
+  <si>
+    <t>0.9246</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.9170</t>
+  </si>
+  <si>
+    <t>0.9086</t>
+  </si>
+  <si>
+    <t>0.9003</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ours (lr 0.001)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>log/Sewer-ML/baseline_resnet18_20251113_134637</t>
+  </si>
+  <si>
+    <t>log/Sewer-ML/baseline_efficientnet_b0_20251113_134832</t>
   </si>
 </sst>
 </file>
@@ -789,7 +925,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +984,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="13"/>
       <color theme="1"/>
@@ -873,8 +1017,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,6 +1041,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,7 +1083,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -944,7 +1102,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,20 +1162,35 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1457,7 +1630,7 @@
       <c r="I3" s="15">
         <v>10.06</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="30">
         <v>65.77</v>
       </c>
       <c r="K3" s="15" t="s">
@@ -1492,7 +1665,7 @@
       <c r="I4" s="15">
         <v>10.51</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="30">
         <v>203.42</v>
       </c>
       <c r="K4" s="15" t="s">
@@ -1527,7 +1700,7 @@
       <c r="I5" s="15">
         <v>17.559999999999999</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="30">
         <v>89.51</v>
       </c>
       <c r="K5" s="15" t="s">
@@ -1562,7 +1735,7 @@
       <c r="I6" s="15">
         <v>8.9600000000000009</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="30">
         <v>60.28</v>
       </c>
       <c r="K6" s="15" t="s">
@@ -1597,7 +1770,7 @@
       <c r="I7" s="15">
         <v>21.07</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="30">
         <v>61.07</v>
       </c>
       <c r="K7" s="15" t="s">
@@ -1632,7 +1805,7 @@
       <c r="I8" s="17">
         <v>3.61</v>
       </c>
-      <c r="J8" s="29">
+      <c r="J8" s="31">
         <v>19.38</v>
       </c>
       <c r="K8" s="15" t="s">
@@ -1653,10 +1826,10 @@
         <v>32</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -1673,10 +1846,10 @@
         <v>130046</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>131</v>
+        <v>117</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -1693,7 +1866,7 @@
         <v>92</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">
@@ -1710,7 +1883,7 @@
         <v>339</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.4">
@@ -1736,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2844C75D-B20C-4DF4-8D50-5B6ECD2343AB}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="86" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A15" zoomScale="86" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1758,7 +1931,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
@@ -1775,7 +1948,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>12</v>
@@ -1804,7 +1977,7 @@
         <v>256</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F3" s="7">
         <v>90</v>
@@ -1829,17 +2002,17 @@
       <c r="C4" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="32">
         <v>64</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F4" s="9">
         <v>90</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>61</v>
@@ -1858,17 +2031,17 @@
       <c r="C5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="32">
         <v>64</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F5" s="9">
         <v>90</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>61</v>
@@ -1887,17 +2060,17 @@
       <c r="C6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="32">
         <v>64</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F6" s="9">
         <v>90</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>61</v>
@@ -1916,17 +2089,17 @@
       <c r="C7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="32">
         <v>64</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F7" s="9">
         <v>90</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>61</v>
@@ -1935,72 +2108,101 @@
         <v>64</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" s="33" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>195</v>
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>62</v>
+      <c r="A11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="8">
+        <v>256</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11" s="7">
+        <v>90</v>
+      </c>
+      <c r="G11" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="A12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="10">
         <v>256</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="E12" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="9">
         <v>90</v>
       </c>
-      <c r="G12" s="8" t="b">
+      <c r="G12" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>63</v>
+      <c r="H12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>70</v>
@@ -2012,7 +2214,7 @@
         <v>256</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F13" s="9">
         <v>90</v>
@@ -2021,15 +2223,15 @@
         <v>0</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>70</v>
@@ -2041,7 +2243,7 @@
         <v>256</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F14" s="9">
         <v>90</v>
@@ -2050,15 +2252,15 @@
         <v>0</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>70</v>
@@ -2070,7 +2272,7 @@
         <v>256</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F15" s="9">
         <v>90</v>
@@ -2079,118 +2281,136 @@
         <v>0</v>
       </c>
       <c r="H15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="8">
+        <v>256</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="7">
+        <v>90</v>
+      </c>
+      <c r="G19" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I19" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="10" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D20" s="10">
         <v>256</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="E20" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="9">
         <v>90</v>
       </c>
-      <c r="G16" s="10" t="b">
+      <c r="G20" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>62</v>
+      <c r="H20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="A21" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="10">
         <v>256</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="7">
+      <c r="E21" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="9">
         <v>90</v>
       </c>
-      <c r="G21" s="8" t="b">
+      <c r="G21" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="H21" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="10" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>70</v>
@@ -2219,7 +2439,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>70</v>
@@ -2240,73 +2460,26 @@
         <v>0</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="10">
-        <v>256</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="9">
-        <v>90</v>
-      </c>
-      <c r="G24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="10">
-        <v>256</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="9">
-        <v>90</v>
-      </c>
-      <c r="G25" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>135</v>
-      </c>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>197</v>
+      <c r="A28" s="33" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
@@ -2323,7 +2496,7 @@
         <v>65</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>12</v>
@@ -2352,7 +2525,7 @@
         <v>256</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F30" s="7">
         <v>90</v>
@@ -2381,7 +2554,7 @@
         <v>256</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F31" s="9">
         <v>90</v>
@@ -2410,7 +2583,7 @@
         <v>256</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F32" s="9">
         <v>90</v>
@@ -2439,7 +2612,7 @@
         <v>256</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F33" s="9">
         <v>90</v>
@@ -2468,7 +2641,7 @@
         <v>256</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F34" s="9">
         <v>90</v>
@@ -2480,186 +2653,7 @@
         <v>61</v>
       </c>
       <c r="I34" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A37" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A39" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="8">
-        <v>256</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F39" s="7">
-        <v>90</v>
-      </c>
-      <c r="G39" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A40" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D40" s="10">
-        <v>256</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="9">
-        <v>90</v>
-      </c>
-      <c r="G40" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A41" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" s="10">
-        <v>256</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="9">
-        <v>90</v>
-      </c>
-      <c r="G41" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A42" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="10">
-        <v>256</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F42" s="9">
-        <v>90</v>
-      </c>
-      <c r="G42" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A43" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="10">
-        <v>256</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="F43" s="9">
-        <v>90</v>
-      </c>
-      <c r="G43" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2669,16 +2663,680 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBD9A2C-CB81-4D62-8BA0-232368B53911}">
+  <dimension ref="A2:K25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="13.8984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" ht="102" x14ac:dyDescent="0.4">
+      <c r="B2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A4" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" s="35">
+        <v>0.6925</v>
+      </c>
+      <c r="C4">
+        <v>51.8</v>
+      </c>
+      <c r="D4">
+        <v>52.21</v>
+      </c>
+      <c r="E4">
+        <v>5221</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>6860</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="27">
+        <v>0.16339999999999999</v>
+      </c>
+      <c r="C5">
+        <v>92.81</v>
+      </c>
+      <c r="D5" s="27">
+        <v>87.61</v>
+      </c>
+      <c r="E5" s="27">
+        <v>9141</v>
+      </c>
+      <c r="F5">
+        <v>8418</v>
+      </c>
+      <c r="G5" s="27">
+        <v>8765</v>
+      </c>
+      <c r="H5">
+        <v>8409</v>
+      </c>
+      <c r="I5" s="27">
+        <v>9136</v>
+      </c>
+      <c r="J5">
+        <v>8757</v>
+      </c>
+      <c r="K5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="27">
+        <v>0.15110000000000001</v>
+      </c>
+      <c r="C6">
+        <v>94.45</v>
+      </c>
+      <c r="D6">
+        <v>87.02</v>
+      </c>
+      <c r="E6">
+        <v>8935</v>
+      </c>
+      <c r="F6">
+        <v>8531</v>
+      </c>
+      <c r="G6">
+        <v>8728</v>
+      </c>
+      <c r="H6">
+        <v>8471</v>
+      </c>
+      <c r="I6">
+        <v>8889</v>
+      </c>
+      <c r="J6">
+        <v>8675</v>
+      </c>
+      <c r="K6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="27">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="C7">
+        <v>94.84</v>
+      </c>
+      <c r="D7" s="27">
+        <v>88.2</v>
+      </c>
+      <c r="E7">
+        <v>8914</v>
+      </c>
+      <c r="F7" s="27">
+        <v>8814</v>
+      </c>
+      <c r="G7" s="27">
+        <v>8864</v>
+      </c>
+      <c r="H7">
+        <v>8720</v>
+      </c>
+      <c r="I7">
+        <v>8827</v>
+      </c>
+      <c r="J7">
+        <v>8773</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="27">
+        <v>0.14319999999999999</v>
+      </c>
+      <c r="C8">
+        <v>95</v>
+      </c>
+      <c r="D8" s="27">
+        <v>87.91</v>
+      </c>
+      <c r="E8">
+        <v>8908</v>
+      </c>
+      <c r="F8">
+        <v>8757</v>
+      </c>
+      <c r="G8" s="27">
+        <v>8832</v>
+      </c>
+      <c r="H8">
+        <v>8667</v>
+      </c>
+      <c r="I8">
+        <v>8827</v>
+      </c>
+      <c r="J8">
+        <v>8746</v>
+      </c>
+      <c r="K8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="27">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="C9">
+        <v>94.53</v>
+      </c>
+      <c r="D9" s="27">
+        <v>87.32</v>
+      </c>
+      <c r="E9">
+        <v>8722</v>
+      </c>
+      <c r="F9" s="27">
+        <v>8870</v>
+      </c>
+      <c r="G9" s="27">
+        <v>8796</v>
+      </c>
+      <c r="H9">
+        <v>8742</v>
+      </c>
+      <c r="I9">
+        <v>8580</v>
+      </c>
+      <c r="J9">
+        <v>8660</v>
+      </c>
+      <c r="K9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A10" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B10" s="35">
+        <v>0.24879999999999999</v>
+      </c>
+      <c r="C10">
+        <v>89.92</v>
+      </c>
+      <c r="D10">
+        <v>87.02</v>
+      </c>
+      <c r="E10">
+        <v>8889</v>
+      </c>
+      <c r="F10">
+        <v>8588</v>
+      </c>
+      <c r="G10">
+        <v>8736</v>
+      </c>
+      <c r="H10">
+        <v>8512</v>
+      </c>
+      <c r="I10">
+        <v>8827</v>
+      </c>
+      <c r="J10">
+        <v>8667</v>
+      </c>
+      <c r="K10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A11" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0.19850000000000001</v>
+      </c>
+      <c r="C11">
+        <v>91.72</v>
+      </c>
+      <c r="D11" s="27">
+        <v>87.61</v>
+      </c>
+      <c r="E11">
+        <v>8729</v>
+      </c>
+      <c r="F11" s="27">
+        <v>8927</v>
+      </c>
+      <c r="G11" s="27">
+        <v>8827</v>
+      </c>
+      <c r="H11">
+        <v>8797</v>
+      </c>
+      <c r="I11">
+        <v>8580</v>
+      </c>
+      <c r="J11">
+        <v>8688</v>
+      </c>
+      <c r="K11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B12" s="27">
+        <v>0.15859999999999999</v>
+      </c>
+      <c r="C12">
+        <v>93.91</v>
+      </c>
+      <c r="D12" s="27">
+        <v>86.43</v>
+      </c>
+      <c r="E12">
+        <v>8830</v>
+      </c>
+      <c r="F12">
+        <v>8531</v>
+      </c>
+      <c r="G12">
+        <v>8678</v>
+      </c>
+      <c r="H12">
+        <v>8452</v>
+      </c>
+      <c r="I12">
+        <v>8765</v>
+      </c>
+      <c r="J12">
+        <v>8606</v>
+      </c>
+      <c r="K12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A13" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13">
+        <v>0.1178</v>
+      </c>
+      <c r="C13">
+        <v>95</v>
+      </c>
+      <c r="D13" s="28">
+        <v>85.55</v>
+      </c>
+      <c r="E13">
+        <v>8596</v>
+      </c>
+      <c r="F13">
+        <v>8644</v>
+      </c>
+      <c r="G13">
+        <v>8620</v>
+      </c>
+      <c r="H13">
+        <v>8509</v>
+      </c>
+      <c r="I13">
+        <v>8457</v>
+      </c>
+      <c r="J13">
+        <v>8483</v>
+      </c>
+      <c r="K13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14">
+        <v>0.1173</v>
+      </c>
+      <c r="C14">
+        <v>95</v>
+      </c>
+      <c r="D14" s="27">
+        <v>87.32</v>
+      </c>
+      <c r="E14">
+        <v>8941</v>
+      </c>
+      <c r="F14">
+        <v>8588</v>
+      </c>
+      <c r="G14">
+        <v>8761</v>
+      </c>
+      <c r="H14">
+        <v>8521</v>
+      </c>
+      <c r="I14">
+        <v>8889</v>
+      </c>
+      <c r="J14">
+        <v>8701</v>
+      </c>
+      <c r="K14" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A15" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15">
+        <v>0.20810000000000001</v>
+      </c>
+      <c r="C15">
+        <v>91.72</v>
+      </c>
+      <c r="D15" s="27">
+        <v>87.32</v>
+      </c>
+      <c r="E15">
+        <v>9036</v>
+      </c>
+      <c r="F15">
+        <v>8475</v>
+      </c>
+      <c r="G15">
+        <v>8746</v>
+      </c>
+      <c r="H15">
+        <v>8439</v>
+      </c>
+      <c r="I15">
+        <v>9012</v>
+      </c>
+      <c r="J15">
+        <v>8716</v>
+      </c>
+      <c r="K15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16">
+        <v>0.1578</v>
+      </c>
+      <c r="C16">
+        <v>94.69</v>
+      </c>
+      <c r="D16" s="27">
+        <v>86.73</v>
+      </c>
+      <c r="E16">
+        <v>8438</v>
+      </c>
+      <c r="F16">
+        <v>9153</v>
+      </c>
+      <c r="G16">
+        <v>8780</v>
+      </c>
+      <c r="H16">
+        <v>8980</v>
+      </c>
+      <c r="I16">
+        <v>8148</v>
+      </c>
+      <c r="J16">
+        <v>8544</v>
+      </c>
+      <c r="K16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="C17">
+        <v>94.38</v>
+      </c>
+      <c r="D17" s="27">
+        <v>86.73</v>
+      </c>
+      <c r="E17">
+        <v>8587</v>
+      </c>
+      <c r="F17">
+        <v>8927</v>
+      </c>
+      <c r="G17">
+        <v>8753</v>
+      </c>
+      <c r="H17">
+        <v>8774</v>
+      </c>
+      <c r="I17">
+        <v>8395</v>
+      </c>
+      <c r="J17">
+        <v>8580</v>
+      </c>
+      <c r="K17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>219</v>
+      </c>
+      <c r="B21">
+        <v>0.14449999999999999</v>
+      </c>
+      <c r="C21">
+        <v>94.77</v>
+      </c>
+      <c r="D21">
+        <v>88.2</v>
+      </c>
+      <c r="E21">
+        <v>8914</v>
+      </c>
+      <c r="F21">
+        <v>8814</v>
+      </c>
+      <c r="G21">
+        <v>8864</v>
+      </c>
+      <c r="H21">
+        <v>8720</v>
+      </c>
+      <c r="I21">
+        <v>8827</v>
+      </c>
+      <c r="J21">
+        <v>8773</v>
+      </c>
+      <c r="K21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22">
+        <v>0.1239</v>
+      </c>
+      <c r="C22">
+        <v>95.47</v>
+      </c>
+      <c r="D22">
+        <v>87.61</v>
+      </c>
+      <c r="E22">
+        <v>8994</v>
+      </c>
+      <c r="F22">
+        <v>8588</v>
+      </c>
+      <c r="G22">
+        <v>8786</v>
+      </c>
+      <c r="H22">
+        <v>8529</v>
+      </c>
+      <c r="I22">
+        <v>8951</v>
+      </c>
+      <c r="J22">
+        <v>8735</v>
+      </c>
+      <c r="K22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>223</v>
+      </c>
+      <c r="K24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>225</v>
+      </c>
+      <c r="K25" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2157F87-0085-4DC7-93EF-26EFA2000176}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="9" width="20.19921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" style="1" customWidth="1"/>
+    <col min="3" max="9" width="20.19921875" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.3984375" style="1" customWidth="1"/>
     <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
@@ -2688,7 +3346,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>155</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -2778,8 +3439,8 @@
       <c r="C4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>101</v>
+      <c r="D4" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="E4" s="5">
         <v>99.85</v>
@@ -2791,7 +3452,7 @@
         <v>0.94579999999999997</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I4" s="1">
         <v>0.91549999999999998</v>
@@ -2820,7 +3481,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E5" s="5">
         <v>99.85</v>
@@ -2861,10 +3522,10 @@
         <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F6" s="1">
         <v>89.97</v>
@@ -2888,7 +3549,7 @@
         <v>0.89629999999999999</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -2902,7 +3563,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" s="1">
         <v>91.65</v>
@@ -2914,13 +3575,13 @@
         <v>0.87709999999999999</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K7" s="1">
         <v>0.86419999999999997</v>
@@ -2932,132 +3593,94 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A9" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A10" s="21" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A11" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B11" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C11" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D11" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H11" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J11" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K11" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="25"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
-        <v>90</v>
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.30220000000000002</v>
-      </c>
-      <c r="E12" s="1">
-        <v>88.67</v>
-      </c>
-      <c r="F12" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>72</v>
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>82</v>
+        <v>23</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>126</v>
+        <v>23</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1">
         <v>90</v>
@@ -3065,40 +3688,40 @@
       <c r="C13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="1">
-        <v>0.21440000000000001</v>
-      </c>
-      <c r="E13" s="1">
-        <v>90.94</v>
-      </c>
-      <c r="F13" s="1">
-        <v>84.37</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>80</v>
+      <c r="D13" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
         <v>90</v>
@@ -3107,39 +3730,39 @@
         <v>70</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="1">
-        <v>91.09</v>
-      </c>
-      <c r="F14" s="1">
-        <v>84.37</v>
+        <v>179</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>88</v>
+        <v>183</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>89</v>
+        <v>184</v>
       </c>
       <c r="M14" s="24" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
         <v>90</v>
@@ -3148,126 +3771,241 @@
         <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="M15" s="24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="61.2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="1">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A21" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C18" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="E18" s="1">
+        <v>94.84</v>
+      </c>
+      <c r="F18" s="1">
+        <v>88.2</v>
+      </c>
+      <c r="G18" s="1">
+        <v>8914</v>
+      </c>
+      <c r="H18" s="1">
+        <v>8814</v>
+      </c>
+      <c r="I18" s="1">
+        <v>8864</v>
+      </c>
+      <c r="J18" s="1">
+        <v>8720</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8827</v>
+      </c>
+      <c r="L18" s="1">
+        <v>8773</v>
+      </c>
+      <c r="M18" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A20" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E20" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="F20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="21" t="s">
+      <c r="G20" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H20" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="I20" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="21" t="s">
+      <c r="J20" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="K20" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M21" s="25"/>
+      <c r="M20" s="25"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="E22" s="1">
+        <v>88.67</v>
+      </c>
+      <c r="F22" s="1">
+        <v>84.37</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>23</v>
+        <v>86</v>
+      </c>
+      <c r="M22" s="24" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>90</v>
@@ -3275,40 +4013,40 @@
       <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>170</v>
+      <c r="D23" s="1">
+        <v>0.21440000000000001</v>
+      </c>
+      <c r="E23" s="1">
+        <v>90.94</v>
+      </c>
+      <c r="F23" s="1">
+        <v>84.37</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>171</v>
+        <v>73</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>172</v>
+        <v>76</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>171</v>
+        <v>77</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>173</v>
+        <v>78</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>173</v>
+        <v>80</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1">
         <v>90</v>
@@ -3317,39 +4055,39 @@
         <v>70</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>164</v>
+        <v>71</v>
+      </c>
+      <c r="E24" s="1">
+        <v>91.09</v>
+      </c>
+      <c r="F24" s="1">
+        <v>84.37</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B25" s="1">
         <v>90</v>
@@ -3358,159 +4096,200 @@
         <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>180</v>
+        <v>186</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>181</v>
+        <v>79</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1">
-        <v>90</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A29" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A30" s="21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C27" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="E27" s="1">
+        <v>94.84</v>
+      </c>
+      <c r="F27" s="1">
+        <v>88.2</v>
+      </c>
+      <c r="G27" s="1">
+        <v>8914</v>
+      </c>
+      <c r="H27" s="1">
+        <v>8814</v>
+      </c>
+      <c r="I27" s="1">
+        <v>8864</v>
+      </c>
+      <c r="J27" s="1">
+        <v>8720</v>
+      </c>
+      <c r="K27" s="1">
+        <v>8827</v>
+      </c>
+      <c r="L27" s="1">
+        <v>8773</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
+      <c r="A29" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B29" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F29" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G29" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="21" t="s">
+      <c r="H29" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="I29" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="21" t="s">
+      <c r="J29" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="21" t="s">
+      <c r="K29" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="L30" s="21" t="s">
+      <c r="L29" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="M30" s="25"/>
+      <c r="M29" s="25"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="B31" s="1">
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>23</v>
+        <v>141</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>23</v>
+        <v>143</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>23</v>
+        <v>145</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>23</v>
+        <v>144</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>23</v>
+        <v>146</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>23</v>
+        <v>146</v>
+      </c>
+      <c r="M31" s="24" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B32" s="1">
         <v>90</v>
@@ -3519,39 +4298,39 @@
         <v>70</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>173</v>
+        <v>135</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1">
         <v>90</v>
@@ -3560,39 +4339,39 @@
         <v>70</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="M33" s="24" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B34" s="1">
         <v>90</v>
@@ -3601,240 +4380,69 @@
         <v>70</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>178</v>
+        <v>126</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="M34" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B35" s="1">
-        <v>90</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M35" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A38" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
-      <c r="A39" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="J39" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="K39" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="L39" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="M39" s="25"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="1">
-        <v>90</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M41" s="24" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A42" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="1">
-        <v>90</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M42" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="1">
-        <v>90</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="M43" s="24" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A44" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B44" s="1">
-        <v>90</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="L44" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M44" s="24" t="s">
-        <v>161</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="C36" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="E36" s="1">
+        <v>94.84</v>
+      </c>
+      <c r="F36" s="1">
+        <v>88.2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>8914</v>
+      </c>
+      <c r="H36" s="1">
+        <v>8814</v>
+      </c>
+      <c r="I36" s="1">
+        <v>8864</v>
+      </c>
+      <c r="J36" s="1">
+        <v>8720</v>
+      </c>
+      <c r="K36" s="1">
+        <v>8827</v>
+      </c>
+      <c r="L36" s="1">
+        <v>8773</v>
+      </c>
+      <c r="M36" s="24" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3842,17 +4450,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="J14" numberStoredAsText="1"/>
+    <ignoredError sqref="J24" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED2E3D2-ADA8-4356-BFE1-6111EA273D35}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.4"/>
@@ -3867,7 +4475,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -3959,7 +4567,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E4" s="11">
         <v>99.93</v>
@@ -3986,7 +4594,7 @@
         <v>0.90949999999999998</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.4">
@@ -4000,7 +4608,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E5" s="11">
         <v>99.09</v>
@@ -4027,7 +4635,7 @@
         <v>0.9244</v>
       </c>
       <c r="M5" s="22" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.4">
@@ -4041,7 +4649,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E6" s="11">
         <v>96.86</v>
@@ -4068,7 +4676,7 @@
         <v>0.91769999999999996</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.4">
@@ -4082,7 +4690,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E7" s="13">
         <v>90.93</v>
@@ -4109,12 +4717,12 @@
         <v>0.90900000000000003</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="12" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -4200,40 +4808,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="M13" s="22" t="s">
-        <v>123</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
@@ -4241,40 +4822,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>190</v>
-      </c>
       <c r="M14" s="22" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
@@ -4282,33 +4836,52 @@
         <v>6</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="M15" s="22" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
-        <v>5</v>
+        <v>236</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
+      <c r="D16" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>230</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" s="12"/>
@@ -4324,7 +4897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083EF1A-8817-41A5-B7D4-F7B8AC6BEDDD}">
   <dimension ref="A1:M16"/>
   <sheetViews>
@@ -4343,7 +4916,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="61.2" x14ac:dyDescent="0.4">
@@ -4434,7 +5007,7 @@
         <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E4" s="1">
         <v>100</v>
@@ -4475,7 +5048,7 @@
         <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1">
         <v>100</v>
@@ -4516,7 +5089,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E6" s="1">
         <v>100</v>
@@ -4557,7 +5130,7 @@
         <v>70</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E7" s="1">
         <v>98.64</v>
@@ -4669,7 +5242,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>70</v>
@@ -4680,7 +5253,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>70</v>
@@ -4691,7 +5264,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>70</v>
@@ -4702,7 +5275,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
🎨refactor: loss 함수 그래프를 train loss에서 val loss로 수정
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannibal\Desktop\cau_cats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319DAB58-875A-4CEF-AA9D-196AAB91C0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D1488A-307B-4394-9A33-7CFC717E999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="660" firstSheet="1" activeTab="2" xr2:uid="{4BF6D8A7-4D2C-4188-8AC2-AA2FABA0E984}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="367">
   <si>
     <t>모델</t>
   </si>
@@ -1248,11 +1248,10 @@
     <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/baseline_xie2019_20251114_023943</t>
   </si>
   <si>
-    <t>nan(Grad Exploding)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Ours (weight_decay 0.0, ps112, drop0.1, res_attn)</t>
+  </si>
+  <si>
+    <t>Ours (weight_decay 0.0, ps112, drop0.1, res_attn)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1292,10 +1291,6 @@
     <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251114_050319</t>
   </si>
   <si>
-    <t>Ours 초기값: adamaWweight_decay 0.01, drop 0.01, feat2, ps56, res_attn false, layers2, patch1, ff_ratio2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>/home/cau/workspace/CHOI/cau_cats/log/Sewer-TAPNEW/run_20251114_051934</t>
   </si>
   <si>
@@ -1330,6 +1325,21 @@
   </si>
   <si>
     <t>xie2019_binary.json</t>
+  </si>
+  <si>
+    <t>Ours 초기값: adamaWweight_decay 0.01, drop 0.01, feat2, ps56, res_attn false, layers2, patch1, ff_ratio2,</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> best_model_criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> best_model_criteria</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>val_loss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2468,11 +2478,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BF4E89-56A3-4502-BA89-E13C3B2DF54B}">
-  <dimension ref="A1:S77"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView zoomScale="84" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N63" sqref="K63:N63"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2483,9 +2493,7 @@
     <col min="4" max="5" width="18.59765625" style="36" customWidth="1"/>
     <col min="6" max="6" width="8" style="36" customWidth="1"/>
     <col min="7" max="7" width="13" style="36" customWidth="1"/>
-    <col min="8" max="9" width="18.59765625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="18.59765625" style="44" customWidth="1"/>
-    <col min="11" max="11" width="18.59765625" style="36" customWidth="1"/>
+    <col min="8" max="11" width="18.59765625" style="36" customWidth="1"/>
     <col min="12" max="17" width="18.59765625" style="44" customWidth="1"/>
     <col min="18" max="16384" width="8.796875" style="36"/>
   </cols>
@@ -2497,7 +2505,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="36" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="62" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
@@ -2528,8 +2536,8 @@
       <c r="I3" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="61" t="s">
-        <v>64</v>
+      <c r="J3" s="60" t="s">
+        <v>365</v>
       </c>
       <c r="K3" s="60" t="s">
         <v>255</v>
@@ -2584,8 +2592,8 @@
       <c r="I4" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="J4" s="49">
-        <v>0.35470000000000002</v>
+      <c r="J4" s="48" t="s">
+        <v>15</v>
       </c>
       <c r="K4" s="48">
         <v>86.14</v>
@@ -2613,9 +2621,6 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J5" s="44" t="s">
-        <v>339</v>
-      </c>
       <c r="K5" s="36">
         <v>78.17</v>
       </c>
@@ -2642,9 +2647,6 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J6" s="44">
-        <v>0.3639</v>
-      </c>
       <c r="K6" s="36">
         <v>84.96</v>
       </c>
@@ -2671,9 +2673,6 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J7" s="44" t="s">
-        <v>339</v>
-      </c>
       <c r="K7" s="36">
         <v>79.650000000000006</v>
       </c>
@@ -2700,9 +2699,6 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="J8" s="44">
-        <v>0.33939999999999998</v>
-      </c>
       <c r="K8" s="36">
         <v>84.96</v>
       </c>
@@ -2756,8 +2752,8 @@
       <c r="I9" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="45">
-        <v>0.18079999999999999</v>
+      <c r="J9" s="41" t="s">
+        <v>258</v>
       </c>
       <c r="K9" s="41">
         <v>86.14</v>
@@ -2794,9 +2790,7 @@
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="37"/>
-      <c r="J10" s="46">
-        <v>0.1424</v>
-      </c>
+      <c r="J10" s="37"/>
       <c r="K10" s="40">
         <v>86.43</v>
       </c>
@@ -2832,9 +2826,7 @@
       <c r="G11" s="37"/>
       <c r="H11" s="37"/>
       <c r="I11" s="37"/>
-      <c r="J11" s="46">
-        <v>0.1152</v>
-      </c>
+      <c r="J11" s="37"/>
       <c r="K11" s="40">
         <v>87.02</v>
       </c>
@@ -2870,9 +2862,7 @@
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="37"/>
-      <c r="J12" s="46">
-        <v>5.0299999999999997E-2</v>
-      </c>
+      <c r="J12" s="37"/>
       <c r="K12" s="40">
         <v>87.02</v>
       </c>
@@ -2908,9 +2898,7 @@
       <c r="G13" s="37"/>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
-      <c r="J13" s="46">
-        <v>0.2276</v>
-      </c>
+      <c r="J13" s="37"/>
       <c r="K13" s="40">
         <v>85.84</v>
       </c>
@@ -2964,8 +2952,8 @@
       <c r="I14" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="45">
-        <v>2.98E-2</v>
+      <c r="J14" s="41" t="s">
+        <v>258</v>
       </c>
       <c r="K14" s="41">
         <v>86.43</v>
@@ -3002,9 +2990,7 @@
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="37"/>
-      <c r="J15" s="46">
-        <v>0.06</v>
-      </c>
+      <c r="J15" s="37"/>
       <c r="K15" s="40">
         <v>89.68</v>
       </c>
@@ -3040,9 +3026,7 @@
       <c r="G16" s="37"/>
       <c r="H16" s="37"/>
       <c r="I16" s="37"/>
-      <c r="J16" s="46">
-        <v>4.6600000000000003E-2</v>
-      </c>
+      <c r="J16" s="37"/>
       <c r="K16" s="40">
         <v>89.09</v>
       </c>
@@ -3069,9 +3053,6 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J17" s="46">
-        <v>6.8400000000000002E-2</v>
-      </c>
       <c r="K17" s="40">
         <v>87.61</v>
       </c>
@@ -3098,9 +3079,6 @@
       </c>
     </row>
     <row r="18" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="J18" s="46">
-        <v>5.5599999999999997E-2</v>
-      </c>
       <c r="K18" s="40">
         <v>87.91</v>
       </c>
@@ -3154,8 +3132,8 @@
       <c r="I19" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J19" s="45">
-        <v>0.22720000000000001</v>
+      <c r="J19" s="41" t="s">
+        <v>258</v>
       </c>
       <c r="K19" s="41">
         <v>85.55</v>
@@ -3192,9 +3170,7 @@
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
-      <c r="J20" s="46">
-        <v>0.22559999999999999</v>
-      </c>
+      <c r="J20" s="40"/>
       <c r="K20" s="40">
         <v>86.43</v>
       </c>
@@ -3221,9 +3197,6 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J21" s="46">
-        <v>0.32279999999999998</v>
-      </c>
       <c r="K21" s="40">
         <v>86.73</v>
       </c>
@@ -3250,9 +3223,6 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J22" s="46">
-        <v>0.32429999999999998</v>
-      </c>
       <c r="K22" s="40">
         <v>82.01</v>
       </c>
@@ -3279,9 +3249,6 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="J23" s="46">
-        <v>0.35299999999999998</v>
-      </c>
       <c r="K23" s="40">
         <v>84.66</v>
       </c>
@@ -3335,8 +3302,8 @@
       <c r="I24" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="45">
-        <v>0.28770000000000001</v>
+      <c r="J24" s="41" t="s">
+        <v>258</v>
       </c>
       <c r="K24" s="41">
         <v>86.14</v>
@@ -3373,9 +3340,7 @@
       <c r="G25" s="40"/>
       <c r="H25" s="40"/>
       <c r="I25" s="40"/>
-      <c r="J25" s="46">
-        <v>0.27810000000000001</v>
-      </c>
+      <c r="J25" s="40"/>
       <c r="K25" s="40">
         <v>85.55</v>
       </c>
@@ -3429,8 +3394,8 @@
       <c r="I26" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="J26" s="46">
-        <v>0.14430000000000001</v>
+      <c r="J26" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K26" s="40">
         <v>87.91</v>
@@ -3467,9 +3432,7 @@
       <c r="G27" s="40"/>
       <c r="H27" s="40"/>
       <c r="I27" s="40"/>
-      <c r="J27" s="46">
-        <v>0.1482</v>
-      </c>
+      <c r="J27" s="40"/>
       <c r="K27" s="40">
         <v>88.2</v>
       </c>
@@ -3505,9 +3468,7 @@
       <c r="G28" s="40"/>
       <c r="H28" s="40"/>
       <c r="I28" s="40"/>
-      <c r="J28" s="46">
-        <v>0.14680000000000001</v>
-      </c>
+      <c r="J28" s="40"/>
       <c r="K28" s="40">
         <v>87.61</v>
       </c>
@@ -3543,9 +3504,7 @@
       <c r="G29" s="40"/>
       <c r="H29" s="40"/>
       <c r="I29" s="40"/>
-      <c r="J29" s="46">
-        <v>0.14280000000000001</v>
-      </c>
+      <c r="J29" s="40"/>
       <c r="K29" s="40">
         <v>87.91</v>
       </c>
@@ -3581,9 +3540,7 @@
       <c r="G30" s="40"/>
       <c r="H30" s="40"/>
       <c r="I30" s="40"/>
-      <c r="J30" s="46">
-        <v>0.14510000000000001</v>
-      </c>
+      <c r="J30" s="40"/>
       <c r="K30" s="40">
         <v>87.91</v>
       </c>
@@ -3637,8 +3594,8 @@
       <c r="I31" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J31" s="46">
-        <v>0.14580000000000001</v>
+      <c r="J31" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K31" s="40">
         <v>88.2</v>
@@ -3675,9 +3632,7 @@
       <c r="G32" s="40"/>
       <c r="H32" s="40"/>
       <c r="I32" s="40"/>
-      <c r="J32" s="46">
-        <v>0.14560000000000001</v>
-      </c>
+      <c r="J32" s="40"/>
       <c r="K32" s="40">
         <v>88.2</v>
       </c>
@@ -3731,8 +3686,8 @@
       <c r="I33" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="46">
-        <v>0.14749999999999999</v>
+      <c r="J33" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K33" s="40">
         <v>88.2</v>
@@ -3769,9 +3724,7 @@
       <c r="G34" s="40"/>
       <c r="H34" s="40"/>
       <c r="I34" s="40"/>
-      <c r="J34" s="46">
-        <v>0.1462</v>
-      </c>
+      <c r="J34" s="40"/>
       <c r="K34" s="40">
         <v>88.2</v>
       </c>
@@ -3825,8 +3778,8 @@
       <c r="I35" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J35" s="46">
-        <v>0.1454</v>
+      <c r="J35" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K35" s="40">
         <v>87.91</v>
@@ -3863,9 +3816,7 @@
       <c r="G36" s="40"/>
       <c r="H36" s="40"/>
       <c r="I36" s="40"/>
-      <c r="J36" s="46">
-        <v>0.14480000000000001</v>
-      </c>
+      <c r="J36" s="40"/>
       <c r="K36" s="40">
         <v>87.91</v>
       </c>
@@ -3919,8 +3870,8 @@
       <c r="I37" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J37" s="46">
-        <v>2.9600000000000001E-2</v>
+      <c r="J37" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K37" s="40">
         <v>87.02</v>
@@ -3957,9 +3908,7 @@
       <c r="G38" s="40"/>
       <c r="H38" s="40"/>
       <c r="I38" s="40"/>
-      <c r="J38" s="46">
-        <v>2.6800000000000001E-2</v>
-      </c>
+      <c r="J38" s="40"/>
       <c r="K38" s="40">
         <v>87.61</v>
       </c>
@@ -4013,8 +3962,8 @@
       <c r="I39" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J39" s="46">
-        <v>0.1459</v>
+      <c r="J39" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K39" s="40">
         <v>86.43</v>
@@ -4051,9 +4000,7 @@
       <c r="G40" s="40"/>
       <c r="H40" s="40"/>
       <c r="I40" s="40"/>
-      <c r="J40" s="46">
-        <v>0.15160000000000001</v>
-      </c>
+      <c r="J40" s="40"/>
       <c r="K40" s="40">
         <v>87.02</v>
       </c>
@@ -4107,8 +4054,8 @@
       <c r="I41" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J41" s="46">
-        <v>0.16520000000000001</v>
+      <c r="J41" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K41" s="40">
         <v>87.32</v>
@@ -4145,9 +4092,7 @@
       <c r="G42" s="40"/>
       <c r="H42" s="40"/>
       <c r="I42" s="40"/>
-      <c r="J42" s="46">
-        <v>0.17</v>
-      </c>
+      <c r="J42" s="40"/>
       <c r="K42" s="40">
         <v>87.91</v>
       </c>
@@ -4201,8 +4146,8 @@
       <c r="I43" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J43" s="46">
-        <v>0.29870000000000002</v>
+      <c r="J43" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K43" s="40">
         <v>86.43</v>
@@ -4257,8 +4202,8 @@
       <c r="I44" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J44" s="46">
-        <v>0.2177</v>
+      <c r="J44" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K44" s="40">
         <v>87.61</v>
@@ -4313,8 +4258,8 @@
       <c r="I45" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J45" s="46">
-        <v>0.2601</v>
+      <c r="J45" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K45" s="40">
         <v>88.2</v>
@@ -4351,9 +4296,7 @@
       <c r="G46" s="40"/>
       <c r="H46" s="40"/>
       <c r="I46" s="40"/>
-      <c r="J46" s="46">
-        <v>0.2611</v>
-      </c>
+      <c r="J46" s="40"/>
       <c r="K46" s="40">
         <v>87.32</v>
       </c>
@@ -4407,8 +4350,8 @@
       <c r="I47" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="J47" s="46">
-        <v>0.19059999999999999</v>
+      <c r="J47" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K47" s="40">
         <v>89.09</v>
@@ -4445,9 +4388,7 @@
       <c r="G48" s="40"/>
       <c r="H48" s="40"/>
       <c r="I48" s="40"/>
-      <c r="J48" s="46">
-        <v>0.18870000000000001</v>
-      </c>
+      <c r="J48" s="40"/>
       <c r="K48" s="40">
         <v>88.79</v>
       </c>
@@ -4501,8 +4442,8 @@
       <c r="I49" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J49" s="46">
-        <v>0.2271</v>
+      <c r="J49" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K49" s="40">
         <v>89.68</v>
@@ -4539,9 +4480,7 @@
       <c r="G50" s="40"/>
       <c r="H50" s="40"/>
       <c r="I50" s="40"/>
-      <c r="J50" s="46">
-        <v>0.2298</v>
-      </c>
+      <c r="J50" s="40"/>
       <c r="K50" s="40">
         <v>89.97</v>
       </c>
@@ -4568,9 +4507,6 @@
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J51" s="46">
-        <v>0.22839999999999999</v>
-      </c>
       <c r="K51" s="40">
         <v>89.68</v>
       </c>
@@ -4597,9 +4533,6 @@
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J52" s="46">
-        <v>0.23019999999999999</v>
-      </c>
       <c r="K52" s="40">
         <v>89.68</v>
       </c>
@@ -4626,9 +4559,6 @@
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J53" s="46">
-        <v>0.23</v>
-      </c>
       <c r="K53" s="40">
         <v>89.97</v>
       </c>
@@ -4682,8 +4612,8 @@
       <c r="I54" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="J54" s="46">
-        <v>0.2465</v>
+      <c r="J54" s="40" t="s">
+        <v>258</v>
       </c>
       <c r="K54" s="40">
         <v>88.5</v>
@@ -4720,9 +4650,7 @@
       <c r="G55" s="40"/>
       <c r="H55" s="40"/>
       <c r="I55" s="40"/>
-      <c r="J55" s="46">
-        <v>0.24579999999999999</v>
-      </c>
+      <c r="J55" s="40"/>
       <c r="K55" s="40">
         <v>89.09</v>
       </c>
@@ -4776,8 +4704,8 @@
       <c r="I56" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J56" s="46">
-        <v>0.27179999999999999</v>
+      <c r="J56" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K56" s="40">
         <v>87.02</v>
@@ -4805,9 +4733,6 @@
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J57" s="46">
-        <v>0.2954</v>
-      </c>
       <c r="K57" s="40">
         <v>87.32</v>
       </c>
@@ -4861,8 +4786,8 @@
       <c r="I58" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="J58" s="46">
-        <v>0.26540000000000002</v>
+      <c r="J58" s="37" t="s">
+        <v>258</v>
       </c>
       <c r="K58" s="40">
         <v>85.25</v>
@@ -4890,9 +4815,6 @@
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J59" s="46">
-        <v>0.2656</v>
-      </c>
       <c r="K59" s="40">
         <v>87.32</v>
       </c>
@@ -4946,8 +4868,8 @@
       <c r="I60" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J60" s="46">
-        <v>0.22989999999999999</v>
+      <c r="J60" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="K60" s="36">
         <v>89.68</v>
@@ -4975,9 +4897,6 @@
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J61" s="44">
-        <v>0.22989999999999999</v>
-      </c>
       <c r="K61" s="36">
         <v>89.68</v>
       </c>
@@ -5031,8 +4950,8 @@
       <c r="I62" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="J62" s="44">
-        <v>0.22570000000000001</v>
+      <c r="J62" s="39" t="s">
+        <v>258</v>
       </c>
       <c r="K62" s="36">
         <v>89.68</v>
@@ -5060,9 +4979,6 @@
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J63" s="44">
-        <v>0.22420000000000001</v>
-      </c>
       <c r="K63" s="36">
         <v>90.27</v>
       </c>
@@ -5089,9 +5005,6 @@
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="J64" s="44">
-        <v>0.22500000000000001</v>
-      </c>
       <c r="K64" s="36">
         <v>89.68</v>
       </c>
@@ -5114,13 +5027,10 @@
         <v>0.89229999999999998</v>
       </c>
       <c r="R64" s="36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J65" s="44">
-        <v>0.22600000000000001</v>
-      </c>
       <c r="K65" s="36">
         <v>89.97</v>
       </c>
@@ -5143,13 +5053,10 @@
         <v>0.89570000000000005</v>
       </c>
       <c r="R65" s="36" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J66" s="44">
-        <v>0.2238</v>
-      </c>
       <c r="K66" s="36">
         <v>89.68</v>
       </c>
@@ -5172,7 +5079,7 @@
         <v>0.89229999999999998</v>
       </c>
       <c r="R66" s="36" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.4">
@@ -5203,8 +5110,8 @@
       <c r="I67" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J67" s="44">
-        <v>0.19919999999999999</v>
+      <c r="J67" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="K67" s="36">
         <v>88.2</v>
@@ -5232,9 +5139,6 @@
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J68" s="44">
-        <v>0.19550000000000001</v>
-      </c>
       <c r="K68" s="36">
         <v>88.5</v>
       </c>
@@ -5289,8 +5193,8 @@
       <c r="I69" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J69" s="44">
-        <v>0.19170000000000001</v>
+      <c r="J69" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="K69" s="36">
         <v>89.09</v>
@@ -5318,9 +5222,6 @@
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J70" s="44">
-        <v>0.1913</v>
-      </c>
       <c r="K70" s="36">
         <v>90.27</v>
       </c>
@@ -5347,9 +5248,6 @@
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J71" s="44">
-        <v>0.191</v>
-      </c>
       <c r="K71" s="36">
         <v>90.27</v>
       </c>
@@ -5372,13 +5270,10 @@
         <v>0.8972</v>
       </c>
       <c r="R71" s="36" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J72" s="44">
-        <v>0.1908</v>
-      </c>
       <c r="K72" s="36">
         <v>89.09</v>
       </c>
@@ -5401,13 +5296,10 @@
         <v>0.88690000000000002</v>
       </c>
       <c r="R72" s="36" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J73" s="44">
-        <v>0.19189999999999999</v>
-      </c>
       <c r="K73" s="36">
         <v>89.38</v>
       </c>
@@ -5430,7 +5322,7 @@
         <v>0.88819999999999999</v>
       </c>
       <c r="R73" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.4">
@@ -5461,8 +5353,8 @@
       <c r="I74" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J74" s="44">
-        <v>0.2165</v>
+      <c r="J74" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="K74" s="36">
         <v>88.5</v>
@@ -5490,9 +5382,6 @@
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J75" s="44">
-        <v>0.2195</v>
-      </c>
       <c r="K75" s="36">
         <v>88.2</v>
       </c>
@@ -5520,7 +5409,7 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A76" s="37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B76" s="36" t="s">
         <v>66</v>
@@ -5546,8 +5435,8 @@
       <c r="I76" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J76" s="44">
-        <v>0.19350000000000001</v>
+      <c r="J76" s="36" t="s">
+        <v>258</v>
       </c>
       <c r="K76" s="36">
         <v>88.79</v>
@@ -5571,13 +5460,10 @@
         <v>0.88049999999999995</v>
       </c>
       <c r="R76" s="36" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="J77" s="44">
-        <v>0.1938</v>
-      </c>
       <c r="K77" s="36">
         <v>89.09</v>
       </c>
@@ -5600,7 +5486,39 @@
         <v>0.88690000000000002</v>
       </c>
       <c r="R77" s="36" t="s">
-        <v>361</v>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A78" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="B78" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="D78" s="36">
+        <v>256</v>
+      </c>
+      <c r="E78" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="F78" s="36">
+        <v>90</v>
+      </c>
+      <c r="G78" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="I78" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J78" s="36" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -5638,7 +5556,7 @@
   <dimension ref="A3:W11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -5651,7 +5569,8 @@
     <col min="7" max="7" width="14.296875" style="53" customWidth="1"/>
     <col min="8" max="8" width="16.59765625" style="53" customWidth="1"/>
     <col min="9" max="9" width="17.296875" style="53" customWidth="1"/>
-    <col min="10" max="18" width="17.796875" style="53" customWidth="1"/>
+    <col min="10" max="10" width="16.59765625" style="53" customWidth="1"/>
+    <col min="11" max="18" width="17.796875" style="53" customWidth="1"/>
     <col min="19" max="16384" width="8.796875" style="53"/>
   </cols>
   <sheetData>
@@ -5684,7 +5603,7 @@
         <v>58</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>64</v>
+        <v>364</v>
       </c>
       <c r="K3" s="51" t="s">
         <v>255</v>
@@ -5740,7 +5659,7 @@
         <v>59</v>
       </c>
       <c r="J4" s="54" t="s">
-        <v>23</v>
+        <v>366</v>
       </c>
       <c r="K4" s="53">
         <v>90.71</v>
@@ -5764,7 +5683,7 @@
         <v>0.90300000000000002</v>
       </c>
       <c r="R4" s="53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S4" s="53"/>
       <c r="T4" s="53"/>
@@ -5800,8 +5719,8 @@
       <c r="I5" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="56">
-        <v>2.2000000000000001E-3</v>
+      <c r="J5" s="54" t="s">
+        <v>15</v>
       </c>
       <c r="K5" s="56">
         <v>91.98</v>
@@ -5897,7 +5816,7 @@
       <c r="I7" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="56"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="56"/>
       <c r="L7" s="56"/>
       <c r="M7" s="56"/>
@@ -5946,7 +5865,7 @@
       <c r="G9" s="54"/>
       <c r="H9" s="54"/>
       <c r="I9" s="54"/>
-      <c r="J9" s="56"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="56"/>
       <c r="L9" s="56"/>
       <c r="M9" s="56"/>
@@ -5966,7 +5885,7 @@
       <c r="G10" s="58"/>
       <c r="H10" s="58"/>
       <c r="I10" s="58"/>
-      <c r="J10" s="54"/>
+      <c r="J10" s="58"/>
       <c r="K10" s="54"/>
       <c r="L10" s="54"/>
       <c r="M10" s="54"/>
@@ -9196,7 +9115,7 @@
         <v>0.91010000000000002</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J7" s="12">
         <v>0.9012</v>

</xml_diff>